<commit_message>
Plotting from LabJack Possible, Export possible, Bug: App does not close with window
</commit_message>
<xml_diff>
--- a/Bachelor/unnamed.xlsx
+++ b/Bachelor/unnamed.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -385,10 +385,8 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C2" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="3">
@@ -396,12 +394,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>5**(1/16)</t>
-        </is>
+        <v>0.1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="4">
@@ -409,12 +405,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>10**(1/16)</t>
-        </is>
+        <v>0.2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="5">
@@ -422,12 +416,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>15**(1/16)</t>
-        </is>
+        <v>0.3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="6">
@@ -435,12 +427,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2**(1/8)*5**(1/16)</t>
-        </is>
+        <v>0.4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="7">
@@ -448,12 +438,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>5**(1/8)</t>
-        </is>
+        <v>0.5</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="8">
@@ -461,12 +449,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>30**(1/16)</t>
-        </is>
+        <v>0.6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="9">
@@ -474,12 +460,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>35**(1/16)</t>
-        </is>
+        <v>0.7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="10">
@@ -487,12 +471,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>40**(1/16)</t>
-        </is>
+        <v>0.7999999999999999</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="11">
@@ -500,12 +482,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>3**(1/8)*5**(1/16)</t>
-        </is>
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="12">
@@ -513,12 +493,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2**(1/16)*5**(1/8)</t>
-        </is>
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="13">
@@ -526,12 +504,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>55**(1/16)</t>
-        </is>
+        <v>1.1</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="14">
@@ -539,12 +515,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>0.6</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>15**(1/16)*2**(1/8)</t>
-        </is>
+        <v>1.2</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
     <row r="15">
@@ -552,12 +526,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>0.65</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>65**(1/16)</t>
-        </is>
+        <v>1.3</v>
+      </c>
+      <c r="C15" t="n">
+        <v>-0.5879884015681682</v>
       </c>
     </row>
     <row r="16">
@@ -565,12 +537,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>70**(1/16)</t>
-        </is>
+        <v>1.4</v>
+      </c>
+      <c r="C16" t="n">
+        <v>-0.23083342490429</v>
       </c>
     </row>
     <row r="17">
@@ -578,12 +548,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>3**(1/16)*5**(1/8)</t>
-        </is>
+        <v>1.5</v>
+      </c>
+      <c r="C17" t="n">
+        <v>-0.4445629679336207</v>
       </c>
     </row>
     <row r="18">
@@ -591,12 +559,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2**(1/4)*5**(1/16)</t>
-        </is>
+        <v>1.6</v>
+      </c>
+      <c r="C18" t="n">
+        <v>-1.427177624282194</v>
       </c>
     </row>
     <row r="19">
@@ -604,12 +570,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>0.85</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>85**(1/16)</t>
-        </is>
+        <v>1.7</v>
+      </c>
+      <c r="C19" t="n">
+        <v>-0.7306089166755783</v>
       </c>
     </row>
     <row r="20">
@@ -617,12 +581,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>10**(1/16)*3**(1/8)</t>
-        </is>
+        <v>1.8</v>
+      </c>
+      <c r="C20" t="n">
+        <v>-1.084539325413061</v>
       </c>
     </row>
     <row r="21">
@@ -630,12 +592,241 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>95**(1/16)</t>
-        </is>
+        <v>1.900000000000001</v>
+      </c>
+      <c r="C21" t="n">
+        <v>-0.9966502726107365</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" t="n">
+        <v>-0.848269066083617</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2.100000000000001</v>
+      </c>
+      <c r="C23" t="n">
+        <v>-0.1776298885321239</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2.200000000000001</v>
+      </c>
+      <c r="C24" t="n">
+        <v>-0.4128318169765635</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2.300000000000001</v>
+      </c>
+      <c r="C25" t="n">
+        <v>-1.205243067321135</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2.400000000000001</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-1.271615134057356</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2.500000000000001</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.1009179963526776</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2.600000000000001</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2.700000000000001</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2.800000000000001</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2.900000000000001</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>3.000000000000001</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>3.100000000000001</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3.200000000000002</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>3.300000000000002</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>3.400000000000002</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>3.500000000000002</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>3.600000000000002</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>3.700000000000002</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>3.800000000000002</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>3.900000000000002</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.01016865175040493</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>4.000000000000002</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.01016865175040493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Better Export and Import, maybe add Info row for resolution, marker (0/1), line(0/1), Color(R, G, B)
</commit_message>
<xml_diff>
--- a/Bachelor/unnamed.xlsx
+++ b/Bachelor/unnamed.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -377,6 +377,21 @@
           <t>y0</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>y1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>y2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>y3</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -386,7 +401,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-1.039691066741943</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="3">
@@ -397,7 +421,16 @@
         <v>0.1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="4">
@@ -408,7 +441,16 @@
         <v>0.2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="5">
@@ -419,7 +461,16 @@
         <v>0.3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="6">
@@ -430,7 +481,16 @@
         <v>0.4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="7">
@@ -441,7 +501,16 @@
         <v>0.5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="8">
@@ -452,7 +521,16 @@
         <v>0.6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="9">
@@ -463,7 +541,16 @@
         <v>0.7</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="10">
@@ -474,7 +561,16 @@
         <v>0.7999999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="11">
@@ -485,7 +581,16 @@
         <v>0.8999999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="12">
@@ -496,7 +601,16 @@
         <v>0.9999999999999999</v>
       </c>
       <c r="C12" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="13">
@@ -507,7 +621,16 @@
         <v>1.1</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="14">
@@ -518,7 +641,16 @@
         <v>1.2</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="15">
@@ -529,7 +661,16 @@
         <v>1.3</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.5879884015681682</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="16">
@@ -540,7 +681,16 @@
         <v>1.4</v>
       </c>
       <c r="C16" t="n">
-        <v>-0.23083342490429</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D16" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E16" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="17">
@@ -551,7 +701,16 @@
         <v>1.5</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.4445629679336207</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E17" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-1.05824089050293</v>
       </c>
     </row>
     <row r="18">
@@ -562,7 +721,16 @@
         <v>1.6</v>
       </c>
       <c r="C18" t="n">
-        <v>-1.427177624282194</v>
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="E18" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="F18" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
     <row r="19">
@@ -573,260 +741,16 @@
         <v>1.7</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.7306089166755783</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="n">
-        <v>18</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="C20" t="n">
-        <v>-1.084539325413061</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1.900000000000001</v>
-      </c>
-      <c r="C21" t="n">
-        <v>-0.9966502726107365</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="B22" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" t="n">
-        <v>-0.848269066083617</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B23" t="n">
-        <v>2.100000000000001</v>
-      </c>
-      <c r="C23" t="n">
-        <v>-0.1776298885321239</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B24" t="n">
-        <v>2.200000000000001</v>
-      </c>
-      <c r="C24" t="n">
-        <v>-0.4128318169765635</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="B25" t="n">
-        <v>2.300000000000001</v>
-      </c>
-      <c r="C25" t="n">
-        <v>-1.205243067321135</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="B26" t="n">
-        <v>2.400000000000001</v>
-      </c>
-      <c r="C26" t="n">
-        <v>-1.271615134057356</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="B27" t="n">
-        <v>2.500000000000001</v>
-      </c>
-      <c r="C27" t="n">
-        <v>-0.1009179963526776</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="B28" t="n">
-        <v>2.600000000000001</v>
-      </c>
-      <c r="C28" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B29" t="n">
-        <v>2.700000000000001</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B30" t="n">
-        <v>2.800000000000001</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="n">
-        <v>2.900000000000001</v>
-      </c>
-      <c r="C31" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="B32" t="n">
-        <v>3.000000000000001</v>
-      </c>
-      <c r="C32" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="B33" t="n">
-        <v>3.100000000000001</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="B34" t="n">
-        <v>3.200000000000002</v>
-      </c>
-      <c r="C34" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="B35" t="n">
-        <v>3.300000000000002</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="B36" t="n">
-        <v>3.400000000000002</v>
-      </c>
-      <c r="C36" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="B37" t="n">
-        <v>3.500000000000002</v>
-      </c>
-      <c r="C37" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="B38" t="n">
-        <v>3.600000000000002</v>
-      </c>
-      <c r="C38" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="B39" t="n">
-        <v>3.700000000000002</v>
-      </c>
-      <c r="C39" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="B40" t="n">
-        <v>3.800000000000002</v>
-      </c>
-      <c r="C40" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="B41" t="n">
-        <v>3.900000000000002</v>
-      </c>
-      <c r="C41" t="n">
-        <v>0.01016865175040493</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="B42" t="n">
-        <v>4.000000000000002</v>
-      </c>
-      <c r="C42" t="n">
-        <v>0.01016865175040493</v>
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="D19" t="n">
+        <v>-1.058248805999756</v>
+      </c>
+      <c r="E19" t="n">
+        <v>-1.05824089050293</v>
+      </c>
+      <c r="F19" t="n">
+        <v>-1.058248805999756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>